<commit_message>
Started prepping for solving
</commit_message>
<xml_diff>
--- a/Excel_Challenge_484 - Pythagorean Triplets for a Sum.xlsx
+++ b/Excel_Challenge_484 - Pythagorean Triplets for a Sum.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75DEC1E7-E108-4C78-A6DB-96266D1FC45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0FA50-2A8A-4798-8FB9-9D4D892DCD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-2850" windowWidth="57840" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-2850" windowWidth="57840" windowHeight="31920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="6">
   <si>
     <t>Answer Expected</t>
   </si>
@@ -340,6 +341,110 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5715</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Thought Bubble: Cloud 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B02BBB3C-2453-4EED-9AA2-8EDBE82CB826}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3729990" y="377190"/>
+          <a:ext cx="4051935" cy="2442210"/>
+        </a:xfrm>
+        <a:prstGeom prst="cloudCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 62422"/>
+            <a:gd name="adj2" fmla="val -29544"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>Pythagorean Triplets follow the rule a^2 + b^2 = c^2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>Find a, b, c where a + b + c = Sum (which is column A).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>So if Sum is 12, then answer is 3, 4, 5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>If there are more than one answer, you can print the first one.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1"/>
+            <a:t>a, b and c are in sorted order.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -605,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -751,4 +856,165 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78CBA6FF-7109-4558-9C4A-A278F4DBF591}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO19" sqref="AO19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>380</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>180</v>
+      </c>
+      <c r="D7">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>546</v>
+      </c>
+      <c r="B8">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>252</v>
+      </c>
+      <c r="D8">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>609</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>644</v>
+      </c>
+      <c r="B10">
+        <v>115</v>
+      </c>
+      <c r="C10">
+        <v>252</v>
+      </c>
+      <c r="D10">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f>115^2+252^2</f>
+        <v>76729</v>
+      </c>
+      <c r="C20">
+        <f>277^2</f>
+        <v>76729</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>